<commit_message>
Agregado de modulo ABMUsuarios
</commit_message>
<xml_diff>
--- a/DB/Planillas para importación Masiva/import_Clientes.xlsx
+++ b/DB/Planillas para importación Masiva/import_Clientes.xlsx
@@ -104,6 +104,21 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
+          <t>Fecha de alta en sistema con el siguiente formato:
+DD/MM/AAAA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
           <t>Dejar siempre en '1'</t>
         </r>
       </text>
@@ -113,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Nombres</t>
   </si>
@@ -140,6 +155,12 @@
   </si>
   <si>
     <t>Estado</t>
+  </si>
+  <si>
+    <t>FechaAlta</t>
+  </si>
+  <si>
+    <t>1/4/2022</t>
   </si>
 </sst>
 </file>
@@ -637,9 +658,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -963,18 +987,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="15" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -994,10 +1016,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +1041,10 @@
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>